<commit_message>
classement des images de pieces et début classe variante perso
</commit_message>
<xml_diff>
--- a/echec/codePieces.xlsx
+++ b/echec/codePieces.xlsx
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -713,7 +713,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="4">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -727,7 +727,7 @@
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -741,7 +741,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="4">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -755,7 +755,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="4">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -769,7 +769,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="4">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>